<commit_message>
updated frequency of occurrence
</commit_message>
<xml_diff>
--- a/Additional Data/WB_Historical_Percent_Occurrence.xlsx
+++ b/Additional Data/WB_Historical_Percent_Occurrence.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26606"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26709"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Taylor/Documents/R Projects/Predator Diets/Additional Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Taylor/Documents/R Projects/Predator-Diets/Additional Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9580" yWindow="460" windowWidth="19220" windowHeight="16580"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$E$121</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$A$121</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -44,9 +44,6 @@
     <t>Benthic Invertebrates</t>
   </si>
   <si>
-    <t>Fish</t>
-  </si>
-  <si>
     <t>type_sum</t>
   </si>
   <si>
@@ -56,13 +53,16 @@
     <t>Spring</t>
   </si>
   <si>
-    <t>Fall</t>
-  </si>
-  <si>
     <t>White Perch</t>
   </si>
   <si>
     <t>Yellow Perch</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>Fish Prey</t>
   </si>
 </sst>
 </file>
@@ -600,6 +600,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -647,12 +650,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -682,12 +685,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -893,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="D110" sqref="D110"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -902,8 +905,9 @@
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
   </cols>
@@ -919,10 +923,10 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -930,13 +934,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>2005</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -947,13 +951,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>2005</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3">
         <v>84.3</v>
@@ -964,13 +968,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>2005</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4">
         <v>35.5</v>
@@ -981,13 +985,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>2005</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5">
         <v>64</v>
@@ -995,16 +999,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>2005</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6">
         <v>6.5</v>
@@ -1012,16 +1016,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>2005</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7">
         <v>4.5</v>
@@ -1032,13 +1036,13 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>2005</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E8">
         <v>78.7</v>
@@ -1049,13 +1053,13 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>2005</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E9">
         <v>30</v>
@@ -1066,13 +1070,13 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10">
         <v>2005</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E10">
         <v>72.7</v>
@@ -1083,13 +1087,13 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <v>2005</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E11">
         <v>70</v>
@@ -1097,16 +1101,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12">
         <v>2005</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E12">
         <v>9.1</v>
@@ -1114,16 +1118,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C13">
         <v>2005</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E13">
         <v>26.6</v>
@@ -1134,13 +1138,13 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C14">
         <v>2006</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14">
         <v>71.7</v>
@@ -1151,13 +1155,13 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C15">
         <v>2006</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15">
         <v>82.9</v>
@@ -1168,13 +1172,13 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C16">
         <v>2006</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E16">
         <v>88.7</v>
@@ -1185,13 +1189,13 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C17">
         <v>2006</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17">
         <v>78</v>
@@ -1199,16 +1203,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C18">
         <v>2006</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E18">
         <v>20.8</v>
@@ -1216,16 +1220,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C19">
         <v>2006</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E19">
         <v>7.3</v>
@@ -1236,13 +1240,13 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C20">
         <v>2006</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E20">
         <v>52</v>
@@ -1253,13 +1257,13 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C21">
         <v>2006</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E21">
         <v>13.6</v>
@@ -1270,13 +1274,13 @@
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C22">
         <v>2006</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E22">
         <v>72</v>
@@ -1287,13 +1291,13 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C23">
         <v>2006</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E23">
         <v>78.2</v>
@@ -1301,16 +1305,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C24">
         <v>2006</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E24">
         <v>60</v>
@@ -1318,16 +1322,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C25">
         <v>2006</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E25">
         <v>34.799999999999997</v>
@@ -1338,13 +1342,13 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C26">
         <v>2007</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E26">
         <v>91.4</v>
@@ -1355,13 +1359,13 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C27">
         <v>2007</v>
       </c>
       <c r="D27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E27">
         <v>60.5</v>
@@ -1372,13 +1376,13 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C28">
         <v>2007</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E28">
         <v>55.2</v>
@@ -1389,13 +1393,13 @@
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C29">
         <v>2007</v>
       </c>
       <c r="D29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E29">
         <v>65.8</v>
@@ -1403,16 +1407,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C30">
         <v>2007</v>
       </c>
       <c r="D30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E30">
         <v>10.3</v>
@@ -1420,16 +1424,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C31">
         <v>2007</v>
       </c>
       <c r="D31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E31">
         <v>2.6</v>
@@ -1440,13 +1444,13 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C32">
         <v>2007</v>
       </c>
       <c r="D32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E32">
         <v>14.3</v>
@@ -1457,13 +1461,13 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C33">
         <v>2007</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -1474,13 +1478,13 @@
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C34">
         <v>2007</v>
       </c>
       <c r="D34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E34">
         <v>47.6</v>
@@ -1491,13 +1495,13 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C35">
         <v>2007</v>
       </c>
       <c r="D35" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E35">
         <v>54.5</v>
@@ -1505,16 +1509,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C36">
         <v>2007</v>
       </c>
       <c r="D36" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E36">
         <v>71.400000000000006</v>
@@ -1522,16 +1526,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C37">
         <v>2007</v>
       </c>
       <c r="D37" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E37">
         <v>54.5</v>
@@ -1542,13 +1546,13 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C38">
         <v>2008</v>
       </c>
       <c r="D38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E38">
         <v>75.599999999999994</v>
@@ -1559,13 +1563,13 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C39">
         <v>2008</v>
       </c>
       <c r="D39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E39">
         <v>30.2</v>
@@ -1576,13 +1580,13 @@
         <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C40">
         <v>2008</v>
       </c>
       <c r="D40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E40">
         <v>41.5</v>
@@ -1593,13 +1597,13 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C41">
         <v>2008</v>
       </c>
       <c r="D41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E41">
         <v>86</v>
@@ -1607,16 +1611,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C42">
         <v>2008</v>
       </c>
       <c r="D42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E42">
         <v>12.2</v>
@@ -1624,16 +1628,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C43">
         <v>2008</v>
       </c>
       <c r="D43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E43">
         <v>23.2</v>
@@ -1644,13 +1648,13 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C44">
         <v>2008</v>
       </c>
       <c r="D44" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E44">
         <v>20</v>
@@ -1661,13 +1665,13 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C45">
         <v>2008</v>
       </c>
       <c r="D45" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E45">
         <v>6.1</v>
@@ -1678,13 +1682,13 @@
         <v>4</v>
       </c>
       <c r="B46" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C46">
         <v>2008</v>
       </c>
       <c r="D46" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E46">
         <v>53.3</v>
@@ -1695,13 +1699,13 @@
         <v>4</v>
       </c>
       <c r="B47" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C47">
         <v>2008</v>
       </c>
       <c r="D47" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E47">
         <v>68.2</v>
@@ -1709,16 +1713,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C48">
         <v>2008</v>
       </c>
       <c r="D48" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E48">
         <v>53.3</v>
@@ -1726,16 +1730,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C49">
         <v>2008</v>
       </c>
       <c r="D49" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E49">
         <v>40.9</v>
@@ -1746,13 +1750,13 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C50">
         <v>2009</v>
       </c>
       <c r="D50" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E50">
         <v>88.4</v>
@@ -1763,13 +1767,13 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C51">
         <v>2009</v>
       </c>
       <c r="D51" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E51">
         <v>42</v>
@@ -1780,13 +1784,13 @@
         <v>4</v>
       </c>
       <c r="B52" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C52">
         <v>2009</v>
       </c>
       <c r="D52" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E52">
         <v>61.6</v>
@@ -1797,13 +1801,13 @@
         <v>4</v>
       </c>
       <c r="B53" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C53">
         <v>2009</v>
       </c>
       <c r="D53" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E53">
         <v>92.9</v>
@@ -1811,16 +1815,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C54">
         <v>2009</v>
       </c>
       <c r="D54" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E54">
         <v>2.2999999999999998</v>
@@ -1828,16 +1832,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C55">
         <v>2009</v>
       </c>
       <c r="D55" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E55">
         <v>14.3</v>
@@ -1848,13 +1852,13 @@
         <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C56">
         <v>2009</v>
       </c>
       <c r="D56" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E56">
         <v>42.4</v>
@@ -1865,13 +1869,13 @@
         <v>1</v>
       </c>
       <c r="B57" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C57">
         <v>2009</v>
       </c>
       <c r="D57" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E57">
         <v>1.3</v>
@@ -1882,13 +1886,13 @@
         <v>4</v>
       </c>
       <c r="B58" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C58">
         <v>2009</v>
       </c>
       <c r="D58" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E58">
         <v>87.9</v>
@@ -1899,13 +1903,13 @@
         <v>4</v>
       </c>
       <c r="B59" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C59">
         <v>2009</v>
       </c>
       <c r="D59" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E59">
         <v>90.7</v>
@@ -1913,16 +1917,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C60">
         <v>2009</v>
       </c>
       <c r="D60" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E60">
         <v>30.3</v>
@@ -1930,16 +1934,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B61" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C61">
         <v>2009</v>
       </c>
       <c r="D61" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E61">
         <v>32</v>
@@ -1950,13 +1954,13 @@
         <v>1</v>
       </c>
       <c r="B62" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C62">
         <v>2010</v>
       </c>
       <c r="D62" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E62">
         <v>88.9</v>
@@ -1967,13 +1971,13 @@
         <v>1</v>
       </c>
       <c r="B63" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C63">
         <v>2010</v>
       </c>
       <c r="D63" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E63">
         <v>70.3</v>
@@ -1984,13 +1988,13 @@
         <v>4</v>
       </c>
       <c r="B64" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C64">
         <v>2010</v>
       </c>
       <c r="D64" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E64">
         <v>61.1</v>
@@ -2001,13 +2005,13 @@
         <v>4</v>
       </c>
       <c r="B65" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C65">
         <v>2010</v>
       </c>
       <c r="D65" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E65">
         <v>87.9</v>
@@ -2015,16 +2019,16 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B66" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C66">
         <v>2010</v>
       </c>
       <c r="D66" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E66">
         <v>20.399999999999999</v>
@@ -2032,16 +2036,16 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C67">
         <v>2010</v>
       </c>
       <c r="D67" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E67">
         <v>25.3</v>
@@ -2052,13 +2056,13 @@
         <v>1</v>
       </c>
       <c r="B68" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C68">
         <v>2010</v>
       </c>
       <c r="D68" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E68">
         <v>59</v>
@@ -2069,13 +2073,13 @@
         <v>1</v>
       </c>
       <c r="B69" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C69">
         <v>2010</v>
       </c>
       <c r="D69" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E69">
         <v>26.8</v>
@@ -2086,13 +2090,13 @@
         <v>4</v>
       </c>
       <c r="B70" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C70">
         <v>2010</v>
       </c>
       <c r="D70" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E70">
         <v>84.6</v>
@@ -2103,13 +2107,13 @@
         <v>4</v>
       </c>
       <c r="B71" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C71">
         <v>2010</v>
       </c>
       <c r="D71" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E71">
         <v>88.7</v>
@@ -2117,16 +2121,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C72">
         <v>2010</v>
       </c>
       <c r="D72" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E72">
         <v>23.1</v>
@@ -2134,16 +2138,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C73">
         <v>2010</v>
       </c>
       <c r="D73" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E73">
         <v>23.9</v>
@@ -2154,13 +2158,13 @@
         <v>1</v>
       </c>
       <c r="B74" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C74">
         <v>2011</v>
       </c>
       <c r="D74" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E74">
         <v>84.6</v>
@@ -2171,13 +2175,13 @@
         <v>1</v>
       </c>
       <c r="B75" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C75">
         <v>2011</v>
       </c>
       <c r="D75" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E75">
         <v>25</v>
@@ -2188,13 +2192,13 @@
         <v>4</v>
       </c>
       <c r="B76" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C76">
         <v>2011</v>
       </c>
       <c r="D76" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E76">
         <v>70.8</v>
@@ -2205,13 +2209,13 @@
         <v>4</v>
       </c>
       <c r="B77" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C77">
         <v>2011</v>
       </c>
       <c r="D77" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E77">
         <v>94.2</v>
@@ -2219,16 +2223,16 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B78" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C78">
         <v>2011</v>
       </c>
       <c r="D78" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E78">
         <v>9.1999999999999993</v>
@@ -2236,16 +2240,16 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B79" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C79">
         <v>2011</v>
       </c>
       <c r="D79" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E79">
         <v>16.3</v>
@@ -2256,13 +2260,13 @@
         <v>1</v>
       </c>
       <c r="B80" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C80">
         <v>2011</v>
       </c>
       <c r="D80" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E80">
         <v>62.3</v>
@@ -2273,13 +2277,13 @@
         <v>1</v>
       </c>
       <c r="B81" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C81">
         <v>2011</v>
       </c>
       <c r="D81" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E81">
         <v>26.8</v>
@@ -2290,13 +2294,13 @@
         <v>4</v>
       </c>
       <c r="B82" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C82">
         <v>2011</v>
       </c>
       <c r="D82" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E82">
         <v>88.3</v>
@@ -2307,13 +2311,13 @@
         <v>4</v>
       </c>
       <c r="B83" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C83">
         <v>2011</v>
       </c>
       <c r="D83" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E83">
         <v>90.2</v>
@@ -2321,16 +2325,16 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B84" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C84">
         <v>2011</v>
       </c>
       <c r="D84" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E84">
         <v>14.3</v>
@@ -2338,16 +2342,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B85" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C85">
         <v>2011</v>
       </c>
       <c r="D85" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E85">
         <v>15.9</v>
@@ -2358,13 +2362,13 @@
         <v>1</v>
       </c>
       <c r="B86" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C86">
         <v>2012</v>
       </c>
       <c r="D86" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E86">
         <v>49.1</v>
@@ -2375,13 +2379,13 @@
         <v>1</v>
       </c>
       <c r="B87" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C87">
         <v>2012</v>
       </c>
       <c r="D87" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E87">
         <v>3.9</v>
@@ -2392,13 +2396,13 @@
         <v>4</v>
       </c>
       <c r="B88" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C88">
         <v>2012</v>
       </c>
       <c r="D88" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E88">
         <v>68.400000000000006</v>
@@ -2409,13 +2413,13 @@
         <v>4</v>
       </c>
       <c r="B89" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C89">
         <v>2012</v>
       </c>
       <c r="D89" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E89">
         <v>94.8</v>
@@ -2423,16 +2427,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B90" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C90">
         <v>2012</v>
       </c>
       <c r="D90" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E90">
         <v>12.3</v>
@@ -2440,16 +2444,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B91" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C91">
         <v>2012</v>
       </c>
       <c r="D91" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E91">
         <v>6.5</v>
@@ -2460,13 +2464,13 @@
         <v>1</v>
       </c>
       <c r="B92" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C92">
         <v>2012</v>
       </c>
       <c r="D92" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E92">
         <v>29</v>
@@ -2477,13 +2481,13 @@
         <v>1</v>
       </c>
       <c r="B93" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C93">
         <v>2012</v>
       </c>
       <c r="D93" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E93">
         <v>3.4</v>
@@ -2494,13 +2498,13 @@
         <v>4</v>
       </c>
       <c r="B94" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C94">
         <v>2012</v>
       </c>
       <c r="D94" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E94">
         <v>22.6</v>
@@ -2511,13 +2515,13 @@
         <v>4</v>
       </c>
       <c r="B95" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C95">
         <v>2012</v>
       </c>
       <c r="D95" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E95">
         <v>71.2</v>
@@ -2525,16 +2529,16 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B96" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C96">
         <v>2012</v>
       </c>
       <c r="D96" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E96">
         <v>54.8</v>
@@ -2542,16 +2546,16 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B97" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C97">
         <v>2012</v>
       </c>
       <c r="D97" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E97">
         <v>37.299999999999997</v>
@@ -2562,13 +2566,13 @@
         <v>1</v>
       </c>
       <c r="B98" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C98">
         <v>2013</v>
       </c>
       <c r="D98" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E98">
         <v>13.5</v>
@@ -2579,13 +2583,13 @@
         <v>1</v>
       </c>
       <c r="B99" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C99">
         <v>2013</v>
       </c>
       <c r="D99" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E99">
         <v>6.5</v>
@@ -2596,13 +2600,13 @@
         <v>4</v>
       </c>
       <c r="B100" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C100">
         <v>2013</v>
       </c>
       <c r="D100" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E100">
         <v>32.6</v>
@@ -2613,13 +2617,13 @@
         <v>4</v>
       </c>
       <c r="B101" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C101">
         <v>2013</v>
       </c>
       <c r="D101" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E101">
         <v>45.5</v>
@@ -2627,16 +2631,16 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B102" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C102">
         <v>2013</v>
       </c>
       <c r="D102" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E102">
         <v>9</v>
@@ -2644,16 +2648,16 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B103" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C103">
         <v>2013</v>
       </c>
       <c r="D103" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E103">
         <v>7.8</v>
@@ -2664,13 +2668,13 @@
         <v>1</v>
       </c>
       <c r="B104" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C104">
         <v>2013</v>
       </c>
       <c r="D104" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E104">
         <v>13.3</v>
@@ -2681,13 +2685,13 @@
         <v>1</v>
       </c>
       <c r="B105" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C105">
         <v>2013</v>
       </c>
       <c r="D105" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E105">
         <v>2.6</v>
@@ -2698,13 +2702,13 @@
         <v>4</v>
       </c>
       <c r="B106" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C106">
         <v>2013</v>
       </c>
       <c r="D106" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E106">
         <v>13.3</v>
@@ -2715,13 +2719,13 @@
         <v>4</v>
       </c>
       <c r="B107" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C107">
         <v>2013</v>
       </c>
       <c r="D107" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E107">
         <v>31.6</v>
@@ -2729,16 +2733,16 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B108" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C108">
         <v>2013</v>
       </c>
       <c r="D108" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E108">
         <v>35.6</v>
@@ -2746,16 +2750,16 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B109" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C109">
         <v>2013</v>
       </c>
       <c r="D109" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E109">
         <v>39.5</v>
@@ -2766,16 +2770,16 @@
         <v>4</v>
       </c>
       <c r="B110" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C110">
         <v>2014</v>
       </c>
       <c r="D110" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E110">
-        <v>182.8</v>
+        <v>89.7</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
@@ -2783,16 +2787,16 @@
         <v>4</v>
       </c>
       <c r="B111" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C111">
         <v>2014</v>
       </c>
       <c r="D111" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E111">
-        <v>228.6</v>
+        <v>94.3</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -2800,16 +2804,16 @@
         <v>4</v>
       </c>
       <c r="B112" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C112">
         <v>2014</v>
       </c>
       <c r="D112" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E112">
-        <v>46.4</v>
+        <v>35.700000000000003</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -2817,30 +2821,30 @@
         <v>4</v>
       </c>
       <c r="B113" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C113">
         <v>2014</v>
       </c>
       <c r="D113" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E113">
-        <v>81.8</v>
+        <v>94.3</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B114" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C114">
         <v>2014</v>
       </c>
       <c r="D114" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E114">
         <v>0</v>
@@ -2848,16 +2852,16 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B115" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C115">
         <v>2014</v>
       </c>
       <c r="D115" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E115">
         <v>22.9</v>
@@ -2865,36 +2869,36 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B116" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C116">
         <v>2014</v>
       </c>
       <c r="D116" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E116">
-        <v>85.7</v>
+        <v>78.599999999999994</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B117" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C117">
         <v>2014</v>
       </c>
       <c r="D117" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E117">
-        <v>39.4</v>
+        <v>33.299999999999997</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -2902,16 +2906,16 @@
         <v>1</v>
       </c>
       <c r="B118" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C118">
         <v>2014</v>
       </c>
       <c r="D118" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E118">
-        <v>106.9</v>
+        <v>62.1</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -2919,16 +2923,16 @@
         <v>1</v>
       </c>
       <c r="B119" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C119">
         <v>2014</v>
       </c>
       <c r="D119" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E119">
-        <v>42.9</v>
+        <v>22.9</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -2936,16 +2940,16 @@
         <v>1</v>
       </c>
       <c r="B120" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C120">
         <v>2014</v>
       </c>
       <c r="D120" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E120">
-        <v>25</v>
+        <v>17.899999999999999</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -2953,13 +2957,13 @@
         <v>1</v>
       </c>
       <c r="B121" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C121">
         <v>2014</v>
       </c>
       <c r="D121" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E121">
         <v>9.1</v>

</xml_diff>